<commit_message>
calculated VPOT PA and CN
</commit_message>
<xml_diff>
--- a/Trabajo Final Pensiones.xlsx
+++ b/Trabajo Final Pensiones.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmond\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hca\Desktop\plan-de-pensiones\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="9113" windowHeight="8220" tabRatio="906" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9120" windowHeight="8220" tabRatio="906" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Preguntas" sheetId="3" r:id="rId1"/>
@@ -378,11 +378,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
     <numFmt numFmtId="165" formatCode="#,##0.000000"/>
-    <numFmt numFmtId="172" formatCode="0.00000000%"/>
+    <numFmt numFmtId="166" formatCode="0.00000000%"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -835,7 +835,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -960,6 +960,7 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -981,11 +982,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1202,7 +1203,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T21"/>
   <sheetViews>
@@ -1210,18 +1211,18 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="2.86328125" customWidth="1"/>
-    <col min="3" max="3" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>29</v>
       </c>
@@ -1229,17 +1230,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D4" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D5" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>33</v>
       </c>
@@ -1247,17 +1248,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D8" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D9" s="12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D10" s="49" t="s">
         <v>59</v>
       </c>
@@ -1271,12 +1272,12 @@
       <c r="L10" s="50"/>
       <c r="M10" s="50"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D11" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>38</v>
       </c>
@@ -1284,95 +1285,95 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D14" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="D15" s="55" t="s">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D15" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="54"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="54"/>
-      <c r="O15" s="54"/>
-      <c r="P15" s="54"/>
-      <c r="Q15" s="54"/>
-      <c r="R15" s="54"/>
-      <c r="S15" s="54"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="54"/>
-      <c r="O16" s="54"/>
-      <c r="P16" s="54"/>
-      <c r="Q16" s="54"/>
-      <c r="R16" s="54"/>
-      <c r="S16" s="54"/>
-    </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="55"/>
+      <c r="M15" s="55"/>
+      <c r="N15" s="55"/>
+      <c r="O15" s="55"/>
+      <c r="P15" s="55"/>
+      <c r="Q15" s="55"/>
+      <c r="R15" s="55"/>
+      <c r="S15" s="55"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="55"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="55"/>
+      <c r="L16" s="55"/>
+      <c r="M16" s="55"/>
+      <c r="N16" s="55"/>
+      <c r="O16" s="55"/>
+      <c r="P16" s="55"/>
+      <c r="Q16" s="55"/>
+      <c r="R16" s="55"/>
+      <c r="S16" s="55"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="54" t="s">
+      <c r="C18" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="54"/>
-      <c r="O18" s="54"/>
-      <c r="P18" s="54"/>
-      <c r="Q18" s="54"/>
-      <c r="R18" s="54"/>
-      <c r="S18" s="54"/>
-      <c r="T18" s="54"/>
-    </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="54"/>
-      <c r="N19" s="54"/>
-      <c r="O19" s="54"/>
-      <c r="P19" s="54"/>
-      <c r="Q19" s="54"/>
-      <c r="R19" s="54"/>
-      <c r="S19" s="54"/>
-      <c r="T19" s="54"/>
-    </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="55"/>
+      <c r="L18" s="55"/>
+      <c r="M18" s="55"/>
+      <c r="N18" s="55"/>
+      <c r="O18" s="55"/>
+      <c r="P18" s="55"/>
+      <c r="Q18" s="55"/>
+      <c r="R18" s="55"/>
+      <c r="S18" s="55"/>
+      <c r="T18" s="55"/>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="55"/>
+      <c r="I19" s="55"/>
+      <c r="J19" s="55"/>
+      <c r="K19" s="55"/>
+      <c r="L19" s="55"/>
+      <c r="M19" s="55"/>
+      <c r="N19" s="55"/>
+      <c r="O19" s="55"/>
+      <c r="P19" s="55"/>
+      <c r="Q19" s="55"/>
+      <c r="R19" s="55"/>
+      <c r="S19" s="55"/>
+      <c r="T19" s="55"/>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>101</v>
       </c>
@@ -1390,26 +1391,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:E167"/>
+  <dimension ref="A1:L167"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E166"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.46484375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1426,7 +1427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1443,7 +1444,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <f>+A3+1</f>
         <v>2</v>
@@ -1461,7 +1462,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" ref="A5:A68" si="0">+A4+1</f>
         <v>3</v>
@@ -1479,7 +1480,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1497,7 +1498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1515,7 +1516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1533,7 +1534,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1551,7 +1552,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1569,7 +1570,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1587,7 +1588,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1605,7 +1606,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1623,7 +1624,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1641,7 +1642,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1659,7 +1660,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1677,7 +1678,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1695,7 +1696,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1712,8 +1713,9 @@
       <c r="E18" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="L18" s="62"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1731,7 +1733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1749,7 +1751,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1767,7 +1769,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1785,7 +1787,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1803,7 +1805,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1821,7 +1823,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1839,7 +1841,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1857,7 +1859,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1875,7 +1877,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1893,7 +1895,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1911,7 +1913,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1929,7 +1931,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1947,7 +1949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1965,7 +1967,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1983,7 +1985,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2001,7 +2003,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -2019,7 +2021,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2037,7 +2039,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2055,7 +2057,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2073,7 +2075,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2091,7 +2093,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2109,7 +2111,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2127,7 +2129,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2145,7 +2147,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2163,7 +2165,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2181,7 +2183,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2199,7 +2201,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2217,7 +2219,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2235,7 +2237,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2253,7 +2255,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2271,7 +2273,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2289,7 +2291,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2307,7 +2309,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2325,7 +2327,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -2343,7 +2345,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -2361,7 +2363,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -2379,7 +2381,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -2397,7 +2399,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -2415,7 +2417,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -2433,7 +2435,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -2451,7 +2453,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -2469,7 +2471,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -2487,7 +2489,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -2505,7 +2507,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -2523,7 +2525,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -2541,7 +2543,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -2559,7 +2561,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -2577,7 +2579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -2595,7 +2597,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -2613,7 +2615,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
         <f t="shared" ref="A69:A132" si="1">+A68+1</f>
         <v>67</v>
@@ -2631,7 +2633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -2649,7 +2651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -2667,7 +2669,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -2685,7 +2687,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -2703,7 +2705,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -2721,7 +2723,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -2739,7 +2741,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -2757,7 +2759,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -2775,7 +2777,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -2793,7 +2795,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>77</v>
@@ -2811,7 +2813,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>78</v>
@@ -2829,7 +2831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -2847,7 +2849,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -2865,7 +2867,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -2883,7 +2885,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -2901,7 +2903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -2919,7 +2921,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -2937,7 +2939,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -2955,7 +2957,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>86</v>
@@ -2973,7 +2975,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -2991,7 +2993,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>88</v>
@@ -3009,7 +3011,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>89</v>
@@ -3027,7 +3029,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -3045,7 +3047,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>91</v>
@@ -3063,7 +3065,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -3081,7 +3083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -3099,7 +3101,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -3117,7 +3119,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -3135,7 +3137,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -3153,7 +3155,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -3171,7 +3173,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -3189,7 +3191,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -3207,7 +3209,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3225,7 +3227,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103">
         <f t="shared" si="1"/>
         <v>101</v>
@@ -3243,7 +3245,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104">
         <f t="shared" si="1"/>
         <v>102</v>
@@ -3261,7 +3263,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105">
         <f t="shared" si="1"/>
         <v>103</v>
@@ -3279,7 +3281,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -3297,7 +3299,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107">
         <f t="shared" si="1"/>
         <v>105</v>
@@ -3315,7 +3317,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -3333,7 +3335,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -3351,7 +3353,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110">
         <f t="shared" si="1"/>
         <v>108</v>
@@ -3369,7 +3371,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -3387,7 +3389,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -3405,7 +3407,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113">
         <f t="shared" si="1"/>
         <v>111</v>
@@ -3423,7 +3425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -3441,7 +3443,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -3459,7 +3461,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116">
         <f t="shared" si="1"/>
         <v>114</v>
@@ -3477,7 +3479,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117">
         <f t="shared" si="1"/>
         <v>115</v>
@@ -3495,7 +3497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118">
         <f t="shared" si="1"/>
         <v>116</v>
@@ -3513,7 +3515,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119">
         <f t="shared" si="1"/>
         <v>117</v>
@@ -3531,7 +3533,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120">
         <f t="shared" si="1"/>
         <v>118</v>
@@ -3549,7 +3551,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121">
         <f t="shared" si="1"/>
         <v>119</v>
@@ -3567,7 +3569,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -3585,7 +3587,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123">
         <f t="shared" si="1"/>
         <v>121</v>
@@ -3603,7 +3605,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124">
         <f t="shared" si="1"/>
         <v>122</v>
@@ -3621,7 +3623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125">
         <f t="shared" si="1"/>
         <v>123</v>
@@ -3639,7 +3641,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126">
         <f t="shared" si="1"/>
         <v>124</v>
@@ -3657,7 +3659,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127">
         <f t="shared" si="1"/>
         <v>125</v>
@@ -3675,7 +3677,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128">
         <f t="shared" si="1"/>
         <v>126</v>
@@ -3693,7 +3695,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129">
         <f t="shared" si="1"/>
         <v>127</v>
@@ -3711,7 +3713,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130">
         <f t="shared" si="1"/>
         <v>128</v>
@@ -3729,7 +3731,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131">
         <f t="shared" si="1"/>
         <v>129</v>
@@ -3747,7 +3749,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132">
         <f t="shared" si="1"/>
         <v>130</v>
@@ -3765,7 +3767,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133">
         <f t="shared" ref="A133:A166" si="2">+A132+1</f>
         <v>131</v>
@@ -3783,7 +3785,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134">
         <f t="shared" si="2"/>
         <v>132</v>
@@ -3801,7 +3803,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135">
         <f t="shared" si="2"/>
         <v>133</v>
@@ -3819,7 +3821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136">
         <f t="shared" si="2"/>
         <v>134</v>
@@ -3837,7 +3839,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137">
         <f t="shared" si="2"/>
         <v>135</v>
@@ -3855,7 +3857,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138">
         <f t="shared" si="2"/>
         <v>136</v>
@@ -3873,7 +3875,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139">
         <f t="shared" si="2"/>
         <v>137</v>
@@ -3891,7 +3893,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140">
         <f t="shared" si="2"/>
         <v>138</v>
@@ -3909,7 +3911,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141">
         <f t="shared" si="2"/>
         <v>139</v>
@@ -3927,7 +3929,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142">
         <f t="shared" si="2"/>
         <v>140</v>
@@ -3945,7 +3947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143">
         <f t="shared" si="2"/>
         <v>141</v>
@@ -3963,7 +3965,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144">
         <f t="shared" si="2"/>
         <v>142</v>
@@ -3981,7 +3983,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145">
         <f t="shared" si="2"/>
         <v>143</v>
@@ -3999,7 +4001,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146">
         <f t="shared" si="2"/>
         <v>144</v>
@@ -4017,7 +4019,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147">
         <f t="shared" si="2"/>
         <v>145</v>
@@ -4035,7 +4037,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148">
         <f t="shared" si="2"/>
         <v>146</v>
@@ -4053,7 +4055,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149">
         <f t="shared" si="2"/>
         <v>147</v>
@@ -4071,7 +4073,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150">
         <f t="shared" si="2"/>
         <v>148</v>
@@ -4089,7 +4091,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151">
         <f t="shared" si="2"/>
         <v>149</v>
@@ -4107,7 +4109,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152">
         <f t="shared" si="2"/>
         <v>150</v>
@@ -4125,7 +4127,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153">
         <f t="shared" si="2"/>
         <v>151</v>
@@ -4143,7 +4145,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154">
         <f t="shared" si="2"/>
         <v>152</v>
@@ -4161,7 +4163,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155">
         <f t="shared" si="2"/>
         <v>153</v>
@@ -4179,7 +4181,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156">
         <f t="shared" si="2"/>
         <v>154</v>
@@ -4197,7 +4199,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157">
         <f t="shared" si="2"/>
         <v>155</v>
@@ -4215,7 +4217,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158">
         <f t="shared" si="2"/>
         <v>156</v>
@@ -4233,7 +4235,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159">
         <f t="shared" si="2"/>
         <v>157</v>
@@ -4251,7 +4253,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160">
         <f t="shared" si="2"/>
         <v>158</v>
@@ -4269,7 +4271,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161">
         <f t="shared" si="2"/>
         <v>159</v>
@@ -4287,7 +4289,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162">
         <f t="shared" si="2"/>
         <v>160</v>
@@ -4305,7 +4307,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163">
         <f t="shared" si="2"/>
         <v>161</v>
@@ -4323,7 +4325,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164">
         <f t="shared" si="2"/>
         <v>162</v>
@@ -4341,7 +4343,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165">
         <f t="shared" si="2"/>
         <v>163</v>
@@ -4359,7 +4361,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166">
         <f t="shared" si="2"/>
         <v>164</v>
@@ -4377,35 +4379,35 @@
         <v>11</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E167" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B2:N51"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="22.53125" customWidth="1"/>
-    <col min="3" max="3" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="11" customWidth="1"/>
-    <col min="10" max="10" width="17.53125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.86328125" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>15</v>
       </c>
@@ -4416,7 +4418,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>17</v>
       </c>
@@ -4427,7 +4429,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>18</v>
       </c>
@@ -4447,7 +4449,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C5" s="3">
         <v>0</v>
       </c>
@@ -4467,7 +4469,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C6" s="3">
         <v>1</v>
       </c>
@@ -4487,7 +4489,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C7" s="3">
         <v>2</v>
       </c>
@@ -4507,7 +4509,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C8" s="3">
         <v>3</v>
       </c>
@@ -4527,7 +4529,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C9" s="3">
         <v>4</v>
       </c>
@@ -4547,7 +4549,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C10" s="3">
         <v>5</v>
       </c>
@@ -4567,7 +4569,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C11" s="3">
         <v>6</v>
       </c>
@@ -4587,7 +4589,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C12" s="3">
         <v>7</v>
       </c>
@@ -4607,7 +4609,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C13" s="3">
         <v>8</v>
       </c>
@@ -4627,7 +4629,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C14" s="3">
         <v>9</v>
       </c>
@@ -4641,7 +4643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C15" s="3">
         <v>10</v>
       </c>
@@ -4655,7 +4657,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C16" s="3">
         <v>11</v>
       </c>
@@ -4672,7 +4674,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C17" s="3">
         <v>12</v>
       </c>
@@ -4689,7 +4691,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C18" s="3">
         <v>13</v>
       </c>
@@ -4709,7 +4711,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="3:14" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="19" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C19" s="3">
         <v>14</v>
       </c>
@@ -4732,7 +4734,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C20" s="3">
         <v>15</v>
       </c>
@@ -4752,7 +4754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C21" s="3">
         <v>16</v>
       </c>
@@ -4772,7 +4774,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C22" s="3">
         <v>17</v>
       </c>
@@ -4792,7 +4794,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C23" s="3">
         <v>18</v>
       </c>
@@ -4812,7 +4814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C24" s="3">
         <v>19</v>
       </c>
@@ -4826,7 +4828,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C25" s="3">
         <v>20</v>
       </c>
@@ -4843,7 +4845,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C26" s="3">
         <v>21</v>
       </c>
@@ -4863,7 +4865,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C27" s="3">
         <v>22</v>
       </c>
@@ -4883,7 +4885,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C28" s="3">
         <v>23</v>
       </c>
@@ -4903,7 +4905,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C29" s="3">
         <v>24</v>
       </c>
@@ -4917,7 +4919,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C30" s="3">
         <v>25</v>
       </c>
@@ -4937,7 +4939,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C31" s="3">
         <v>26</v>
       </c>
@@ -4951,7 +4953,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C32" s="3">
         <v>27</v>
       </c>
@@ -4965,7 +4967,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C33" s="3">
         <v>28</v>
       </c>
@@ -4979,7 +4981,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C34" s="3">
         <v>29</v>
       </c>
@@ -4993,7 +4995,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C35" s="3">
         <v>30</v>
       </c>
@@ -5007,7 +5009,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C36" s="3">
         <v>31</v>
       </c>
@@ -5021,7 +5023,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C37" s="3">
         <v>32</v>
       </c>
@@ -5035,7 +5037,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C38" s="3">
         <v>33</v>
       </c>
@@ -5049,7 +5051,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C39" s="3">
         <v>34</v>
       </c>
@@ -5063,7 +5065,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C40" s="3">
         <v>35</v>
       </c>
@@ -5077,7 +5079,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C41" s="3">
         <v>36</v>
       </c>
@@ -5091,7 +5093,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C42" s="3">
         <v>37</v>
       </c>
@@ -5105,7 +5107,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C43" s="3">
         <v>38</v>
       </c>
@@ -5119,7 +5121,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C44" s="3">
         <v>39</v>
       </c>
@@ -5133,7 +5135,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C45" s="3">
         <v>40</v>
       </c>
@@ -5147,7 +5149,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="2:6" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B47" s="8" t="s">
         <v>22</v>
       </c>
@@ -5155,7 +5157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:3" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" s="8" t="s">
         <v>23</v>
       </c>
@@ -5163,7 +5165,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="2:3" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B51" s="8" t="s">
         <v>24</v>
       </c>
@@ -5177,21 +5179,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B3:F60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>68</v>
       </c>
@@ -5199,7 +5201,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>66</v>
       </c>
@@ -5207,7 +5209,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>67</v>
       </c>
@@ -5215,15 +5217,15 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E6" s="14"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>65</v>
       </c>
@@ -5240,7 +5242,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" s="16">
         <v>15</v>
       </c>
@@ -5257,7 +5259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="19">
         <v>16</v>
       </c>
@@ -5274,7 +5276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="19">
         <v>17</v>
       </c>
@@ -5291,7 +5293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" s="19">
         <v>18</v>
       </c>
@@ -5308,7 +5310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" s="19">
         <v>19</v>
       </c>
@@ -5325,7 +5327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="19">
         <v>20</v>
       </c>
@@ -5342,7 +5344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" s="19">
         <v>21</v>
       </c>
@@ -5359,7 +5361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="19">
         <v>22</v>
       </c>
@@ -5376,7 +5378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" s="19">
         <v>23</v>
       </c>
@@ -5393,7 +5395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" s="19">
         <v>24</v>
       </c>
@@ -5410,7 +5412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" s="19">
         <v>25</v>
       </c>
@@ -5427,7 +5429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" s="19">
         <v>26</v>
       </c>
@@ -5444,7 +5446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="19">
         <v>27</v>
       </c>
@@ -5461,7 +5463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" s="19">
         <v>28</v>
       </c>
@@ -5478,7 +5480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" s="19">
         <v>29</v>
       </c>
@@ -5495,7 +5497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25" s="19">
         <v>30</v>
       </c>
@@ -5512,7 +5514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" s="19">
         <v>31</v>
       </c>
@@ -5529,7 +5531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" s="19">
         <v>32</v>
       </c>
@@ -5546,7 +5548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" s="19">
         <v>33</v>
       </c>
@@ -5563,7 +5565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" s="19">
         <v>34</v>
       </c>
@@ -5580,7 +5582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B30" s="19">
         <v>35</v>
       </c>
@@ -5597,7 +5599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" s="19">
         <v>36</v>
       </c>
@@ -5614,7 +5616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B32" s="19">
         <v>37</v>
       </c>
@@ -5631,7 +5633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" s="19">
         <v>38</v>
       </c>
@@ -5648,7 +5650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" s="19">
         <v>39</v>
       </c>
@@ -5665,7 +5667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" s="19">
         <v>40</v>
       </c>
@@ -5682,7 +5684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" s="19">
         <v>41</v>
       </c>
@@ -5699,7 +5701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" s="19">
         <v>42</v>
       </c>
@@ -5716,7 +5718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" s="19">
         <v>43</v>
       </c>
@@ -5733,7 +5735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" s="19">
         <v>44</v>
       </c>
@@ -5750,7 +5752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" s="19">
         <v>45</v>
       </c>
@@ -5767,7 +5769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" s="19">
         <v>46</v>
       </c>
@@ -5784,7 +5786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B42" s="19">
         <v>47</v>
       </c>
@@ -5801,7 +5803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B43" s="19">
         <v>48</v>
       </c>
@@ -5818,7 +5820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B44" s="19">
         <v>49</v>
       </c>
@@ -5835,7 +5837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B45" s="19">
         <v>50</v>
       </c>
@@ -5852,7 +5854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B46" s="19">
         <v>51</v>
       </c>
@@ -5869,7 +5871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B47" s="19">
         <v>52</v>
       </c>
@@ -5886,7 +5888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B48" s="19">
         <v>53</v>
       </c>
@@ -5903,7 +5905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B49" s="19">
         <v>54</v>
       </c>
@@ -5920,7 +5922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B50" s="19">
         <v>55</v>
       </c>
@@ -5937,7 +5939,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B51" s="19">
         <v>56</v>
       </c>
@@ -5954,7 +5956,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B52" s="19">
         <v>57</v>
       </c>
@@ -5971,7 +5973,7 @@
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B53" s="19">
         <v>58</v>
       </c>
@@ -5988,7 +5990,7 @@
         <v>9.375E-2</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B54" s="19">
         <v>59</v>
       </c>
@@ -6005,7 +6007,7 @@
         <v>0.10575</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B55" s="19">
         <v>60</v>
       </c>
@@ -6022,7 +6024,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B56" s="19">
         <v>61</v>
       </c>
@@ -6039,7 +6041,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B57" s="19">
         <v>62</v>
       </c>
@@ -6056,7 +6058,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B58" s="19">
         <v>63</v>
       </c>
@@ -6073,7 +6075,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B59" s="19">
         <v>64</v>
       </c>
@@ -6090,7 +6092,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="60" spans="2:6" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B60" s="22">
         <v>65</v>
       </c>
@@ -6113,7 +6115,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:O18"/>
   <sheetViews>
@@ -6121,30 +6123,30 @@
       <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="9" max="13" width="33.33203125" customWidth="1"/>
-    <col min="15" max="15" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="9" max="13" width="33.28515625" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="13.15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:15" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:15" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="56" t="s">
+      <c r="I2" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="J2" s="58" t="s">
+      <c r="J2" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="60"/>
-    </row>
-    <row r="3" spans="2:15" ht="40.9" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="61"/>
+    </row>
+    <row r="3" spans="2:15" ht="43.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="36" t="s">
         <v>70</v>
       </c>
@@ -6154,7 +6156,7 @@
       <c r="D3" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="I3" s="57"/>
+      <c r="I3" s="58"/>
       <c r="J3" s="39" t="s">
         <v>43</v>
       </c>
@@ -6168,7 +6170,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="27.4" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="27">
         <v>0</v>
       </c>
@@ -6194,7 +6196,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="13.9" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="30">
         <v>496.08</v>
       </c>
@@ -6220,7 +6222,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="27.4" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="32">
         <v>4210.42</v>
       </c>
@@ -6246,7 +6248,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="15.4" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="32">
         <v>7399.43</v>
       </c>
@@ -6272,7 +6274,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="15.4" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="32">
         <v>8601.51</v>
       </c>
@@ -6298,7 +6300,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="15.4" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="32">
         <v>10298.36</v>
       </c>
@@ -6323,9 +6325,9 @@
       <c r="M9" s="42">
         <v>0.01</v>
       </c>
-      <c r="O9" s="61"/>
-    </row>
-    <row r="10" spans="2:15" ht="37.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O9" s="54"/>
+    </row>
+    <row r="10" spans="2:15" ht="37.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="32">
         <v>20770.3</v>
       </c>
@@ -6351,7 +6353,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="13.9" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="32">
         <v>32736.84</v>
       </c>
@@ -6362,7 +6364,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:15" ht="13.9" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="32">
         <v>62500.01</v>
       </c>
@@ -6373,7 +6375,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="13.9" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="32">
         <v>83333.34</v>
       </c>
@@ -6384,7 +6386,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="13.9" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="33">
         <v>250000</v>
       </c>
@@ -6398,22 +6400,22 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="I15" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="I16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I17" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="48"/>
       <c r="I18" t="s">
         <v>97</v>
@@ -6429,7 +6431,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CE21519-DB50-4F23-886E-3BAAC6692D6A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:F166"/>
   <sheetViews>
@@ -6437,20 +6439,20 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.9296875" customWidth="1"/>
-    <col min="2" max="2" width="18.46484375" customWidth="1"/>
-    <col min="3" max="3" width="13.1328125" customWidth="1"/>
-    <col min="4" max="4" width="18.73046875" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="51" t="s">
         <v>104</v>
       </c>
@@ -6470,7 +6472,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="51">
         <v>1</v>
       </c>
@@ -6487,7 +6489,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="51">
         <f>+A3+1</f>
         <v>2</v>
@@ -6505,7 +6507,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="51">
         <f t="shared" ref="A5:A68" si="0">+A4+1</f>
         <v>3</v>
@@ -6523,7 +6525,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="51">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -6541,7 +6543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="51">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -6559,7 +6561,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="51">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6577,7 +6579,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="51">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -6595,7 +6597,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="51">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -6613,7 +6615,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="51">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -6631,7 +6633,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="51">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -6649,7 +6651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="51">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -6667,7 +6669,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="51">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -6685,7 +6687,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="51">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -6703,7 +6705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="51">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -6721,7 +6723,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="51">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -6739,7 +6741,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="51">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -6757,7 +6759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="51">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -6775,7 +6777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="51">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -6793,7 +6795,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="51">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -6811,7 +6813,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="51">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6829,7 +6831,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="51">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -6847,7 +6849,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="51">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -6865,7 +6867,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="51">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -6883,7 +6885,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="51">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -6901,7 +6903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="51">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -6919,7 +6921,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="51">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -6937,7 +6939,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="51">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -6955,7 +6957,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="51">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -6973,7 +6975,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="51">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -6991,7 +6993,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="51">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -7009,7 +7011,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="51">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -7027,7 +7029,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="51">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -7045,7 +7047,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="51">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -7063,7 +7065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="51">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -7081,7 +7083,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="51">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -7099,7 +7101,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="51">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -7117,7 +7119,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="51">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -7135,7 +7137,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="51">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -7153,7 +7155,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="51">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -7171,7 +7173,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="51">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -7189,7 +7191,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="51">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -7207,7 +7209,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="51">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -7225,7 +7227,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="51">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -7243,7 +7245,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="51">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -7261,7 +7263,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="51">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -7279,7 +7281,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="51">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -7297,7 +7299,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="51">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -7315,7 +7317,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="51">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -7333,7 +7335,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="51">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -7351,7 +7353,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="51">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -7369,7 +7371,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="51">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -7387,7 +7389,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="51">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -7405,7 +7407,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="51">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -7423,7 +7425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="51">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -7441,7 +7443,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="51">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -7459,7 +7461,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="51">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -7477,7 +7479,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="51">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -7495,7 +7497,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="51">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -7513,7 +7515,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="51">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -7531,7 +7533,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="51">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -7549,7 +7551,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="51">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -7567,7 +7569,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="51">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -7585,7 +7587,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="51">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -7603,7 +7605,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="51">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -7621,7 +7623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="51">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -7639,7 +7641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="51">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -7657,7 +7659,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="51">
         <f t="shared" ref="A69:A132" si="1">+A68+1</f>
         <v>67</v>
@@ -7675,7 +7677,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="51">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -7693,7 +7695,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="51">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -7711,7 +7713,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="51">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -7729,7 +7731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="51">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -7747,7 +7749,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="51">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -7765,7 +7767,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="51">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -7783,7 +7785,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="51">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -7801,7 +7803,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="51">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -7819,7 +7821,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="51">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -7837,7 +7839,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="51">
         <f t="shared" si="1"/>
         <v>77</v>
@@ -7855,7 +7857,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="51">
         <f t="shared" si="1"/>
         <v>78</v>
@@ -7873,7 +7875,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="51">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -7891,7 +7893,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="51">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -7909,7 +7911,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="51">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -7927,7 +7929,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="51">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -7945,7 +7947,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="51">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -7963,7 +7965,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="51">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -7981,7 +7983,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="51">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -7999,7 +8001,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="51">
         <f t="shared" si="1"/>
         <v>86</v>
@@ -8017,7 +8019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="51">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -8035,7 +8037,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="51">
         <f t="shared" si="1"/>
         <v>88</v>
@@ -8053,7 +8055,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="51">
         <f t="shared" si="1"/>
         <v>89</v>
@@ -8071,7 +8073,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="51">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -8089,7 +8091,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="51">
         <f t="shared" si="1"/>
         <v>91</v>
@@ -8107,7 +8109,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="51">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -8125,7 +8127,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="51">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -8143,7 +8145,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="51">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -8161,7 +8163,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="51">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -8179,7 +8181,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="51">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -8197,7 +8199,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="51">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -8215,7 +8217,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="51">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -8233,7 +8235,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="51">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -8251,7 +8253,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="51">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -8269,7 +8271,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="51">
         <f t="shared" si="1"/>
         <v>101</v>
@@ -8287,7 +8289,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="51">
         <f t="shared" si="1"/>
         <v>102</v>
@@ -8305,7 +8307,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="51">
         <f t="shared" si="1"/>
         <v>103</v>
@@ -8323,7 +8325,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="51">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -8341,7 +8343,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="51">
         <f t="shared" si="1"/>
         <v>105</v>
@@ -8359,7 +8361,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="51">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -8377,7 +8379,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="51">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -8395,7 +8397,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="51">
         <f t="shared" si="1"/>
         <v>108</v>
@@ -8413,7 +8415,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="51">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -8431,7 +8433,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="51">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -8449,7 +8451,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="51">
         <f t="shared" si="1"/>
         <v>111</v>
@@ -8467,7 +8469,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="51">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -8485,7 +8487,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="51">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -8503,7 +8505,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="51">
         <f t="shared" si="1"/>
         <v>114</v>
@@ -8521,7 +8523,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="51">
         <f t="shared" si="1"/>
         <v>115</v>
@@ -8539,7 +8541,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="51">
         <f t="shared" si="1"/>
         <v>116</v>
@@ -8557,7 +8559,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="51">
         <f t="shared" si="1"/>
         <v>117</v>
@@ -8575,7 +8577,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="51">
         <f t="shared" si="1"/>
         <v>118</v>
@@ -8593,7 +8595,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="51">
         <f t="shared" si="1"/>
         <v>119</v>
@@ -8611,7 +8613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="51">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -8629,7 +8631,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="51">
         <f t="shared" si="1"/>
         <v>121</v>
@@ -8647,7 +8649,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="51">
         <f t="shared" si="1"/>
         <v>122</v>
@@ -8665,7 +8667,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="51">
         <f t="shared" si="1"/>
         <v>123</v>
@@ -8683,7 +8685,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="51">
         <f t="shared" si="1"/>
         <v>124</v>
@@ -8701,7 +8703,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="51">
         <f t="shared" si="1"/>
         <v>125</v>
@@ -8719,7 +8721,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="51">
         <f t="shared" si="1"/>
         <v>126</v>
@@ -8737,7 +8739,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="51">
         <f t="shared" si="1"/>
         <v>127</v>
@@ -8755,7 +8757,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="51">
         <f t="shared" si="1"/>
         <v>128</v>
@@ -8773,7 +8775,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="51">
         <f t="shared" si="1"/>
         <v>129</v>
@@ -8791,7 +8793,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="51">
         <f t="shared" si="1"/>
         <v>130</v>
@@ -8809,7 +8811,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="51">
         <f t="shared" ref="A133:A166" si="2">+A132+1</f>
         <v>131</v>
@@ -8827,7 +8829,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="51">
         <f t="shared" si="2"/>
         <v>132</v>
@@ -8845,7 +8847,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="51">
         <f t="shared" si="2"/>
         <v>133</v>
@@ -8863,7 +8865,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="51">
         <f t="shared" si="2"/>
         <v>134</v>
@@ -8881,7 +8883,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="51">
         <f t="shared" si="2"/>
         <v>135</v>
@@ -8899,7 +8901,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="51">
         <f t="shared" si="2"/>
         <v>136</v>
@@ -8917,7 +8919,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="51">
         <f t="shared" si="2"/>
         <v>137</v>
@@ -8935,7 +8937,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="51">
         <f t="shared" si="2"/>
         <v>138</v>
@@ -8953,7 +8955,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="51">
         <f t="shared" si="2"/>
         <v>139</v>
@@ -8971,7 +8973,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="51">
         <f t="shared" si="2"/>
         <v>140</v>
@@ -8989,7 +8991,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="51">
         <f t="shared" si="2"/>
         <v>141</v>
@@ -9007,7 +9009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="51">
         <f t="shared" si="2"/>
         <v>142</v>
@@ -9025,7 +9027,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="51">
         <f t="shared" si="2"/>
         <v>143</v>
@@ -9043,7 +9045,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="51">
         <f t="shared" si="2"/>
         <v>144</v>
@@ -9061,7 +9063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="51">
         <f t="shared" si="2"/>
         <v>145</v>
@@ -9079,7 +9081,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="51">
         <f t="shared" si="2"/>
         <v>146</v>
@@ -9097,7 +9099,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="51">
         <f t="shared" si="2"/>
         <v>147</v>
@@ -9115,7 +9117,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="51">
         <f t="shared" si="2"/>
         <v>148</v>
@@ -9133,7 +9135,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="51">
         <f t="shared" si="2"/>
         <v>149</v>
@@ -9151,7 +9153,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="51">
         <f t="shared" si="2"/>
         <v>150</v>
@@ -9169,7 +9171,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="51">
         <f t="shared" si="2"/>
         <v>151</v>
@@ -9187,7 +9189,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="51">
         <f t="shared" si="2"/>
         <v>152</v>
@@ -9205,7 +9207,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="51">
         <f t="shared" si="2"/>
         <v>153</v>
@@ -9223,7 +9225,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="51">
         <f t="shared" si="2"/>
         <v>154</v>
@@ -9241,7 +9243,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="51">
         <f t="shared" si="2"/>
         <v>155</v>
@@ -9259,7 +9261,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="51">
         <f t="shared" si="2"/>
         <v>156</v>
@@ -9277,7 +9279,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="51">
         <f t="shared" si="2"/>
         <v>157</v>
@@ -9295,7 +9297,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="51">
         <f t="shared" si="2"/>
         <v>158</v>
@@ -9313,7 +9315,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="51">
         <f t="shared" si="2"/>
         <v>159</v>
@@ -9331,7 +9333,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="51">
         <f t="shared" si="2"/>
         <v>160</v>
@@ -9349,7 +9351,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="51">
         <f t="shared" si="2"/>
         <v>161</v>
@@ -9367,7 +9369,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="51">
         <f t="shared" si="2"/>
         <v>162</v>
@@ -9385,7 +9387,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="51">
         <f t="shared" si="2"/>
         <v>163</v>
@@ -9403,7 +9405,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="51">
         <f t="shared" si="2"/>
         <v>164</v>
@@ -9427,15 +9429,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Lista_x0020_de_x0020_Categor_x00ed_as xmlns="9A05114E-EDEA-4799-9DBB-DF8668FB4C19" xsi:nil="true"/>
-    <Categor_x00ed_a xmlns="9A05114E-EDEA-4799-9DBB-DF8668FB4C19" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100DAAB1EA61EA8B744B09F1F7EB2E27C2C" ma:contentTypeVersion="" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="048623a67e90a2dcbb561f93f6ce966d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9A05114E-EDEA-4799-9DBB-DF8668FB4C19" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1ee9541165358530c0f167d6b0e5567" ns2:_="">
     <xsd:import namespace="9A05114E-EDEA-4799-9DBB-DF8668FB4C19"/>
@@ -9569,6 +9562,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Lista_x0020_de_x0020_Categor_x00ed_as xmlns="9A05114E-EDEA-4799-9DBB-DF8668FB4C19" xsi:nil="true"/>
+    <Categor_x00ed_a xmlns="9A05114E-EDEA-4799-9DBB-DF8668FB4C19" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -9579,22 +9581,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A8B3AF5-60D2-43C4-A7F5-F0CCC7FC668C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="9A05114E-EDEA-4799-9DBB-DF8668FB4C19"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE5EE63E-C8D0-4043-971B-64F2F45F5B2E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9612,6 +9598,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A8B3AF5-60D2-43C4-A7F5-F0CCC7FC668C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="9A05114E-EDEA-4799-9DBB-DF8668FB4C19"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE01A233-3C64-47BB-B608-78678EDB9071}">
   <ds:schemaRefs>

</xml_diff>